<commit_message>
Fix home table for Table 3 levels
</commit_message>
<xml_diff>
--- a/Taxonomy_tables_v3.2.xlsx
+++ b/Taxonomy_tables_v3.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anirudh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cye/Documents/wip/gem_taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC20F9D-3D54-0542-A3E8-A85E0C43AC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AD23FB-D539-4E4B-A7E8-B48676B0CE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="780" windowWidth="28800" windowHeight="17540" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taxonomy v3.2" sheetId="1" r:id="rId1"/>
@@ -2933,12 +2933,6 @@
     <t>* Type of lateral load-resisting system</t>
   </si>
   <si>
-    <t>System ductility (Level 1)</t>
-  </si>
-  <si>
-    <t>Seismic code level (Level 2)</t>
-  </si>
-  <si>
     <t>Columns-Wall density (Level 3)</t>
   </si>
   <si>
@@ -3279,9 +3273,6 @@
   </si>
   <si>
     <t>Table from Taxonomy v2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Lateral load coefficcient (Level 2.1)</t>
   </si>
   <si>
     <t>Lateral load coefficcient</t>
@@ -3392,6 +3383,15 @@
   </si>
   <si>
     <t>DUH</t>
+  </si>
+  <si>
+    <t>Seismic code level (Level 1)</t>
+  </si>
+  <si>
+    <t>System ductility (Level 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Lateral load coefficcient (Level 1.1)</t>
   </si>
 </sst>
 </file>
@@ -5182,14 +5182,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5200,32 +5197,65 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5251,41 +5281,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5478,12 +5478,12 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38097" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -5829,7 +5829,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -5846,43 +5846,43 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="199" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="212" t="s">
+      <c r="A3" s="200" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="213" t="s">
+      <c r="B3" s="201" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="212" t="s">
+      <c r="C3" s="200" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="212" t="s">
+      <c r="D3" s="200" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="212" t="s">
+      <c r="E3" s="200" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="212" t="s">
+      <c r="G3" s="200" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="212"/>
-      <c r="B4" s="213"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
-      <c r="G4" s="212"/>
+      <c r="A4" s="200"/>
+      <c r="B4" s="201"/>
+      <c r="C4" s="200"/>
+      <c r="D4" s="200"/>
+      <c r="E4" s="200"/>
+      <c r="F4" s="200"/>
+      <c r="G4" s="200"/>
     </row>
     <row r="5" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="204" t="s">
+      <c r="A5" s="203" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="188">
@@ -5895,7 +5895,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="187" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F5" s="187" t="s">
         <v>10</v>
@@ -5905,150 +5905,150 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="204"/>
-      <c r="B6" s="203">
+      <c r="A6" s="203"/>
+      <c r="B6" s="202">
         <v>2</v>
       </c>
-      <c r="C6" s="204" t="s">
+      <c r="C6" s="203" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="205" t="s">
+      <c r="D6" s="204" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="187" t="s">
         <v>850</v>
       </c>
-      <c r="F6" s="204" t="s">
+      <c r="F6" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="204" t="s">
+      <c r="G6" s="203" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="204"/>
-      <c r="B7" s="203"/>
-      <c r="C7" s="204"/>
-      <c r="D7" s="205"/>
+      <c r="A7" s="203"/>
+      <c r="B7" s="202"/>
+      <c r="C7" s="203"/>
+      <c r="D7" s="204"/>
       <c r="E7" s="187" t="s">
         <v>846</v>
       </c>
-      <c r="F7" s="204"/>
-      <c r="G7" s="204"/>
+      <c r="F7" s="203"/>
+      <c r="G7" s="203"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="204"/>
-      <c r="B8" s="203"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="205"/>
+      <c r="A8" s="203"/>
+      <c r="B8" s="202"/>
+      <c r="C8" s="203"/>
+      <c r="D8" s="204"/>
       <c r="E8" s="187" t="s">
-        <v>878</v>
-      </c>
-      <c r="F8" s="204"/>
-      <c r="G8" s="204"/>
+        <v>876</v>
+      </c>
+      <c r="F8" s="203"/>
+      <c r="G8" s="203"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="204"/>
-      <c r="B9" s="203"/>
-      <c r="C9" s="204"/>
-      <c r="D9" s="205"/>
+      <c r="A9" s="203"/>
+      <c r="B9" s="202"/>
+      <c r="C9" s="203"/>
+      <c r="D9" s="204"/>
       <c r="E9" s="187" t="s">
         <v>848</v>
       </c>
-      <c r="F9" s="204"/>
-      <c r="G9" s="204"/>
+      <c r="F9" s="203"/>
+      <c r="G9" s="203"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="204"/>
-      <c r="B10" s="203">
+      <c r="A10" s="203"/>
+      <c r="B10" s="202">
         <v>3</v>
       </c>
-      <c r="C10" s="204" t="s">
+      <c r="C10" s="203" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="205" t="s">
+      <c r="D10" s="204" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="187" t="s">
         <v>851</v>
       </c>
-      <c r="F10" s="204" t="s">
+      <c r="F10" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="204" t="s">
+      <c r="G10" s="203" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="204"/>
-      <c r="B11" s="203"/>
-      <c r="C11" s="204"/>
-      <c r="D11" s="205"/>
+      <c r="A11" s="203"/>
+      <c r="B11" s="202"/>
+      <c r="C11" s="203"/>
+      <c r="D11" s="204"/>
       <c r="E11" s="187" t="s">
+        <v>970</v>
+      </c>
+      <c r="F11" s="203"/>
+      <c r="G11" s="203"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="203"/>
+      <c r="B12" s="202"/>
+      <c r="C12" s="203"/>
+      <c r="D12" s="204"/>
+      <c r="E12" s="187" t="s">
+        <v>972</v>
+      </c>
+      <c r="F12" s="203"/>
+      <c r="G12" s="203"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="203"/>
+      <c r="B13" s="202"/>
+      <c r="C13" s="203"/>
+      <c r="D13" s="204"/>
+      <c r="E13" s="187" t="s">
+        <v>971</v>
+      </c>
+      <c r="F13" s="203"/>
+      <c r="G13" s="203"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="203"/>
+      <c r="B14" s="202"/>
+      <c r="C14" s="203"/>
+      <c r="D14" s="204"/>
+      <c r="E14" s="187" t="s">
         <v>852</v>
       </c>
-      <c r="F11" s="204"/>
-      <c r="G11" s="204"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="204"/>
-      <c r="B12" s="203"/>
-      <c r="C12" s="204"/>
-      <c r="D12" s="205"/>
-      <c r="E12" s="187" t="s">
+      <c r="F14" s="203"/>
+      <c r="G14" s="203"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="203"/>
+      <c r="B15" s="202"/>
+      <c r="C15" s="203"/>
+      <c r="D15" s="204"/>
+      <c r="E15" s="187" t="s">
         <v>853</v>
       </c>
-      <c r="F12" s="204"/>
-      <c r="G12" s="204"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="204"/>
-      <c r="B13" s="203"/>
-      <c r="C13" s="204"/>
-      <c r="D13" s="205"/>
-      <c r="E13" s="187" t="s">
-        <v>958</v>
-      </c>
-      <c r="F13" s="204"/>
-      <c r="G13" s="204"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="204"/>
-      <c r="B14" s="203"/>
-      <c r="C14" s="204"/>
-      <c r="D14" s="205"/>
-      <c r="E14" s="187" t="s">
+      <c r="F15" s="203"/>
+      <c r="G15" s="203"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="203" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="205">
+        <v>4</v>
+      </c>
+      <c r="C16" s="208" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="211" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="187" t="s">
         <v>854</v>
-      </c>
-      <c r="F14" s="204"/>
-      <c r="G14" s="204"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="204"/>
-      <c r="B15" s="203"/>
-      <c r="C15" s="204"/>
-      <c r="D15" s="205"/>
-      <c r="E15" s="187" t="s">
-        <v>855</v>
-      </c>
-      <c r="F15" s="204"/>
-      <c r="G15" s="204"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="204" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="208">
-        <v>4</v>
-      </c>
-      <c r="C16" s="200" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="206" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="187" t="s">
-        <v>856</v>
       </c>
       <c r="F16" s="187" t="s">
         <v>19</v>
@@ -6058,27 +6058,27 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="204"/>
-      <c r="B17" s="211"/>
-      <c r="C17" s="201"/>
-      <c r="D17" s="210"/>
+      <c r="A17" s="203"/>
+      <c r="B17" s="206"/>
+      <c r="C17" s="209"/>
+      <c r="D17" s="212"/>
       <c r="E17" s="187" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="F17" s="187" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="G17" s="187">
         <v>22.6</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="204"/>
-      <c r="B18" s="211"/>
-      <c r="C18" s="201"/>
-      <c r="D18" s="210"/>
+      <c r="A18" s="203"/>
+      <c r="B18" s="206"/>
+      <c r="C18" s="209"/>
+      <c r="D18" s="212"/>
       <c r="E18" s="187" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="F18" s="187" t="s">
         <v>19</v>
@@ -6088,48 +6088,48 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="204"/>
-      <c r="B19" s="211"/>
-      <c r="C19" s="201"/>
-      <c r="D19" s="210"/>
+      <c r="A19" s="203"/>
+      <c r="B19" s="206"/>
+      <c r="C19" s="209"/>
+      <c r="D19" s="212"/>
       <c r="E19" s="187" t="s">
+        <v>857</v>
+      </c>
+      <c r="F19" s="191" t="s">
         <v>859</v>
-      </c>
-      <c r="F19" s="191" t="s">
-        <v>861</v>
       </c>
       <c r="G19" s="187">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="204"/>
-      <c r="B20" s="209"/>
-      <c r="C20" s="202"/>
-      <c r="D20" s="207"/>
+      <c r="A20" s="203"/>
+      <c r="B20" s="207"/>
+      <c r="C20" s="210"/>
+      <c r="D20" s="213"/>
       <c r="E20" s="187" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="F20" s="187" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="G20" s="187">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="204"/>
-      <c r="B21" s="208">
+      <c r="A21" s="203"/>
+      <c r="B21" s="205">
         <v>5</v>
       </c>
-      <c r="C21" s="200" t="s">
+      <c r="C21" s="208" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="205" t="s">
+      <c r="D21" s="204" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="187" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="F21" s="187" t="s">
         <v>19</v>
@@ -6139,12 +6139,12 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="204"/>
-      <c r="B22" s="209"/>
-      <c r="C22" s="202"/>
-      <c r="D22" s="205"/>
+      <c r="A22" s="203"/>
+      <c r="B22" s="207"/>
+      <c r="C22" s="210"/>
+      <c r="D22" s="204"/>
       <c r="E22" s="187" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="F22" s="187" t="s">
         <v>10</v>
@@ -6152,52 +6152,52 @@
       <c r="G22" s="187"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="204"/>
-      <c r="B23" s="203">
+      <c r="A23" s="203"/>
+      <c r="B23" s="202">
         <v>6</v>
       </c>
-      <c r="C23" s="204" t="s">
+      <c r="C23" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="206" t="s">
+      <c r="D23" s="211" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="187" t="s">
-        <v>868</v>
-      </c>
-      <c r="F23" s="204" t="s">
+        <v>866</v>
+      </c>
+      <c r="F23" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="204" t="s">
+      <c r="G23" s="203" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="204"/>
-      <c r="B24" s="203"/>
-      <c r="C24" s="204"/>
-      <c r="D24" s="207"/>
+      <c r="A24" s="203"/>
+      <c r="B24" s="202"/>
+      <c r="C24" s="203"/>
+      <c r="D24" s="213"/>
       <c r="E24" s="187" t="s">
         <v>849</v>
       </c>
-      <c r="F24" s="204"/>
-      <c r="G24" s="204"/>
+      <c r="F24" s="203"/>
+      <c r="G24" s="203"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="204" t="s">
+      <c r="A25" s="203" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="208">
+      <c r="B25" s="205">
         <v>7</v>
       </c>
-      <c r="C25" s="200" t="s">
+      <c r="C25" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="206" t="s">
+      <c r="D25" s="211" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="187" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="F25" s="187" t="s">
         <v>10</v>
@@ -6207,12 +6207,12 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="204"/>
-      <c r="B26" s="209"/>
-      <c r="C26" s="202"/>
-      <c r="D26" s="207"/>
+      <c r="A26" s="203"/>
+      <c r="B26" s="207"/>
+      <c r="C26" s="210"/>
+      <c r="D26" s="213"/>
       <c r="E26" s="187" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="F26" s="187" t="s">
         <v>10</v>
@@ -6222,72 +6222,72 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="204"/>
-      <c r="B27" s="203">
+      <c r="A27" s="203"/>
+      <c r="B27" s="202">
         <v>8</v>
       </c>
-      <c r="C27" s="204" t="s">
+      <c r="C27" s="203" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="206" t="s">
+      <c r="D27" s="211" t="s">
         <v>28</v>
       </c>
       <c r="E27" s="187" t="s">
-        <v>871</v>
-      </c>
-      <c r="F27" s="204" t="s">
+        <v>869</v>
+      </c>
+      <c r="F27" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="204" t="s">
+      <c r="G27" s="203" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="204"/>
-      <c r="B28" s="203"/>
-      <c r="C28" s="204"/>
-      <c r="D28" s="210"/>
+      <c r="A28" s="203"/>
+      <c r="B28" s="202"/>
+      <c r="C28" s="203"/>
+      <c r="D28" s="212"/>
       <c r="E28" s="187" t="s">
+        <v>873</v>
+      </c>
+      <c r="F28" s="203"/>
+      <c r="G28" s="203"/>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A29" s="203"/>
+      <c r="B29" s="202"/>
+      <c r="C29" s="203"/>
+      <c r="D29" s="212"/>
+      <c r="E29" s="187" t="s">
+        <v>874</v>
+      </c>
+      <c r="F29" s="203"/>
+      <c r="G29" s="203"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="203"/>
+      <c r="B30" s="202"/>
+      <c r="C30" s="203"/>
+      <c r="D30" s="212"/>
+      <c r="E30" s="187" t="s">
+        <v>870</v>
+      </c>
+      <c r="F30" s="203"/>
+      <c r="G30" s="203"/>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A31" s="203"/>
+      <c r="B31" s="202"/>
+      <c r="C31" s="203"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="187" t="s">
         <v>875</v>
       </c>
-      <c r="F28" s="204"/>
-      <c r="G28" s="204"/>
-    </row>
-    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="204"/>
-      <c r="B29" s="203"/>
-      <c r="C29" s="204"/>
-      <c r="D29" s="210"/>
-      <c r="E29" s="187" t="s">
-        <v>876</v>
-      </c>
-      <c r="F29" s="204"/>
-      <c r="G29" s="204"/>
-    </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="204"/>
-      <c r="B30" s="203"/>
-      <c r="C30" s="204"/>
-      <c r="D30" s="210"/>
-      <c r="E30" s="187" t="s">
-        <v>872</v>
-      </c>
-      <c r="F30" s="204"/>
-      <c r="G30" s="204"/>
-    </row>
-    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A31" s="204"/>
-      <c r="B31" s="203"/>
-      <c r="C31" s="204"/>
-      <c r="D31" s="207"/>
-      <c r="E31" s="187" t="s">
-        <v>877</v>
-      </c>
-      <c r="F31" s="204"/>
-      <c r="G31" s="204"/>
+      <c r="F31" s="203"/>
+      <c r="G31" s="203"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="204"/>
+      <c r="A32" s="203"/>
       <c r="B32" s="188">
         <v>9</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="187" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="F32" s="187" t="s">
         <v>10</v>
@@ -6309,18 +6309,18 @@
       <c r="I32" s="193"/>
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="204"/>
-      <c r="B33" s="208">
+      <c r="A33" s="203"/>
+      <c r="B33" s="205">
         <v>10</v>
       </c>
-      <c r="C33" s="200" t="s">
+      <c r="C33" s="208" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="206" t="s">
+      <c r="D33" s="211" t="s">
         <v>33</v>
       </c>
       <c r="E33" s="187" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="F33" s="187" t="s">
         <v>10</v>
@@ -6331,12 +6331,12 @@
       <c r="I33" s="193"/>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="204"/>
-      <c r="B34" s="211"/>
-      <c r="C34" s="201"/>
-      <c r="D34" s="210"/>
+      <c r="A34" s="203"/>
+      <c r="B34" s="206"/>
+      <c r="C34" s="209"/>
+      <c r="D34" s="212"/>
       <c r="E34" s="187" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="F34" s="187" t="s">
         <v>10</v>
@@ -6347,12 +6347,12 @@
       <c r="I34" s="193"/>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="204"/>
-      <c r="B35" s="209"/>
-      <c r="C35" s="202"/>
-      <c r="D35" s="207"/>
+      <c r="A35" s="203"/>
+      <c r="B35" s="207"/>
+      <c r="C35" s="210"/>
+      <c r="D35" s="213"/>
       <c r="E35" s="187" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="F35" s="187" t="s">
         <v>10</v>
@@ -6362,87 +6362,87 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="200" t="s">
+      <c r="A36" s="208" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="203">
+      <c r="B36" s="202">
         <v>11</v>
       </c>
-      <c r="C36" s="204" t="s">
+      <c r="C36" s="203" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="205" t="s">
+      <c r="D36" s="204" t="s">
         <v>39</v>
       </c>
       <c r="E36" s="187" t="s">
+        <v>878</v>
+      </c>
+      <c r="F36" s="203" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="203" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="209"/>
+      <c r="B37" s="202"/>
+      <c r="C37" s="203"/>
+      <c r="D37" s="204"/>
+      <c r="E37" s="187" t="s">
+        <v>879</v>
+      </c>
+      <c r="F37" s="203"/>
+      <c r="G37" s="203"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="209"/>
+      <c r="B38" s="202"/>
+      <c r="C38" s="203"/>
+      <c r="D38" s="204"/>
+      <c r="E38" s="187" t="s">
         <v>880</v>
       </c>
-      <c r="F36" s="204" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="204" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="201"/>
-      <c r="B37" s="203"/>
-      <c r="C37" s="204"/>
-      <c r="D37" s="205"/>
-      <c r="E37" s="187" t="s">
+      <c r="F38" s="203"/>
+      <c r="G38" s="203"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="209"/>
+      <c r="B39" s="202"/>
+      <c r="C39" s="203"/>
+      <c r="D39" s="204"/>
+      <c r="E39" s="187" t="s">
         <v>881</v>
       </c>
-      <c r="F37" s="204"/>
-      <c r="G37" s="204"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="201"/>
-      <c r="B38" s="203"/>
-      <c r="C38" s="204"/>
-      <c r="D38" s="205"/>
-      <c r="E38" s="187" t="s">
+      <c r="F39" s="203"/>
+      <c r="G39" s="203"/>
+    </row>
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A40" s="209"/>
+      <c r="B40" s="202"/>
+      <c r="C40" s="203"/>
+      <c r="D40" s="204"/>
+      <c r="E40" s="187" t="s">
         <v>882</v>
       </c>
-      <c r="F38" s="204"/>
-      <c r="G38" s="204"/>
-    </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="201"/>
-      <c r="B39" s="203"/>
-      <c r="C39" s="204"/>
-      <c r="D39" s="205"/>
-      <c r="E39" s="187" t="s">
-        <v>883</v>
-      </c>
-      <c r="F39" s="204"/>
-      <c r="G39" s="204"/>
-    </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="201"/>
-      <c r="B40" s="203"/>
-      <c r="C40" s="204"/>
-      <c r="D40" s="205"/>
-      <c r="E40" s="187" t="s">
-        <v>884</v>
-      </c>
-      <c r="F40" s="204"/>
-      <c r="G40" s="204"/>
+      <c r="F40" s="203"/>
+      <c r="G40" s="203"/>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="201"/>
-      <c r="B41" s="203">
+      <c r="A41" s="209"/>
+      <c r="B41" s="202">
         <v>12</v>
       </c>
-      <c r="C41" s="204" t="s">
+      <c r="C41" s="203" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="205" t="s">
+      <c r="D41" s="204" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="187" t="s">
-        <v>864</v>
-      </c>
-      <c r="F41" s="204" t="s">
+        <v>862</v>
+      </c>
+      <c r="F41" s="203" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="187" t="s">
@@ -6450,29 +6450,29 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="201"/>
-      <c r="B42" s="203"/>
-      <c r="C42" s="204"/>
-      <c r="D42" s="205"/>
+      <c r="A42" s="209"/>
+      <c r="B42" s="202"/>
+      <c r="C42" s="203"/>
+      <c r="D42" s="204"/>
       <c r="E42" s="187" t="s">
-        <v>865</v>
-      </c>
-      <c r="F42" s="204"/>
+        <v>863</v>
+      </c>
+      <c r="F42" s="203"/>
       <c r="G42" s="187"/>
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="201"/>
-      <c r="B43" s="203"/>
-      <c r="C43" s="204"/>
-      <c r="D43" s="205"/>
+      <c r="A43" s="209"/>
+      <c r="B43" s="202"/>
+      <c r="C43" s="203"/>
+      <c r="D43" s="204"/>
       <c r="E43" s="187" t="s">
-        <v>879</v>
-      </c>
-      <c r="F43" s="204"/>
+        <v>877</v>
+      </c>
+      <c r="F43" s="203"/>
       <c r="G43" s="187"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="201"/>
+      <c r="A44" s="209"/>
       <c r="B44" s="188">
         <v>13</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>42</v>
       </c>
       <c r="E44" s="187" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="F44" s="187" t="s">
         <v>10</v>
@@ -6493,7 +6493,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="202"/>
+      <c r="A45" s="210"/>
       <c r="B45" s="188">
         <v>14</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>833</v>
       </c>
       <c r="E45" s="187" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="F45" s="187" t="s">
         <v>10</v>
@@ -6513,18 +6513,31 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A36:A45"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
     <mergeCell ref="F10:F15"/>
     <mergeCell ref="G10:G15"/>
     <mergeCell ref="A16:A24"/>
@@ -6540,31 +6553,18 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="A25:A35"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
@@ -6660,7 +6660,7 @@
         <v>809</v>
       </c>
       <c r="C5" s="244" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.2">
@@ -6668,7 +6668,7 @@
         <v>812</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C6" s="245"/>
     </row>
@@ -6677,7 +6677,7 @@
         <v>813</v>
       </c>
       <c r="B7" s="116" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C7" s="245"/>
     </row>
@@ -6686,7 +6686,7 @@
         <v>814</v>
       </c>
       <c r="B8" s="116" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C8" s="245"/>
     </row>
@@ -6695,7 +6695,7 @@
         <v>815</v>
       </c>
       <c r="B9" s="116" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C9" s="246"/>
     </row>
@@ -7046,7 +7046,7 @@
         <v>816</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.2">
@@ -7063,7 +7063,7 @@
         <v>817</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
@@ -7080,7 +7080,7 @@
         <v>818</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
@@ -7254,7 +7254,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>44</v>
@@ -7272,7 +7272,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>44</v>
@@ -7328,7 +7328,7 @@
         <v>751</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -7444,7 +7444,7 @@
         <v>612</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -7467,7 +7467,7 @@
         <v>622</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>627</v>
@@ -7632,13 +7632,13 @@
         <v>751</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>654</v>
       </c>
       <c r="H17" s="102" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="I17" s="143"/>
       <c r="J17" s="149"/>
@@ -7658,7 +7658,7 @@
         <v>655</v>
       </c>
       <c r="H18" s="102" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="I18" s="249"/>
       <c r="J18" s="248"/>
@@ -7672,7 +7672,7 @@
         <v>656</v>
       </c>
       <c r="H19" s="102" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="I19" s="249"/>
       <c r="J19" s="248"/>
@@ -7806,7 +7806,7 @@
         <v>672</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="I27" s="143"/>
       <c r="J27" s="149"/>
@@ -8548,7 +8548,7 @@
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="184" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -8741,8 +8741,8 @@
       </c>
       <c r="C5" s="102"/>
       <c r="D5" s="151"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="223"/>
+      <c r="E5" s="232"/>
+      <c r="F5" s="220"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -8757,8 +8757,8 @@
       <c r="D6" s="174" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="224"/>
-      <c r="F6" s="223"/>
+      <c r="E6" s="219"/>
+      <c r="F6" s="220"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -8773,8 +8773,8 @@
       <c r="D7" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="225"/>
-      <c r="F7" s="226"/>
+      <c r="E7" s="221"/>
+      <c r="F7" s="222"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -8789,8 +8789,8 @@
       <c r="D8" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="225"/>
-      <c r="F8" s="226"/>
+      <c r="E8" s="221"/>
+      <c r="F8" s="222"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
@@ -8805,8 +8805,8 @@
       <c r="D9" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="225"/>
-      <c r="F9" s="226"/>
+      <c r="E9" s="221"/>
+      <c r="F9" s="222"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="120"/>
@@ -8817,8 +8817,8 @@
       <c r="D10" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="227"/>
-      <c r="F10" s="228"/>
+      <c r="E10" s="223"/>
+      <c r="F10" s="224"/>
     </row>
     <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
@@ -8841,8 +8841,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="224"/>
-      <c r="B12" s="223"/>
+      <c r="A12" s="219"/>
+      <c r="B12" s="220"/>
       <c r="C12" s="151" t="s">
         <v>99</v>
       </c>
@@ -8857,8 +8857,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="225"/>
-      <c r="B13" s="226"/>
+      <c r="A13" s="221"/>
+      <c r="B13" s="222"/>
       <c r="C13" s="151" t="s">
         <v>103</v>
       </c>
@@ -8873,8 +8873,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="227"/>
-      <c r="B14" s="228"/>
+      <c r="A14" s="223"/>
+      <c r="B14" s="224"/>
       <c r="C14" s="151" t="s">
         <v>107</v>
       </c>
@@ -8901,8 +8901,8 @@
       <c r="D15" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="224"/>
-      <c r="F15" s="223"/>
+      <c r="E15" s="219"/>
+      <c r="F15" s="220"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="163"/>
@@ -8913,8 +8913,8 @@
       <c r="D16" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="225"/>
-      <c r="F16" s="226"/>
+      <c r="E16" s="221"/>
+      <c r="F16" s="222"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="164"/>
@@ -8925,8 +8925,8 @@
       <c r="D17" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="227"/>
-      <c r="F17" s="228"/>
+      <c r="E17" s="223"/>
+      <c r="F17" s="224"/>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
@@ -9410,15 +9410,15 @@
     </row>
     <row r="51" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>965</v>
-      </c>
-      <c r="C51" s="233" t="s">
-        <v>964</v>
-      </c>
-      <c r="D51" s="234"/>
+        <v>962</v>
+      </c>
+      <c r="C51" s="217" t="s">
+        <v>961</v>
+      </c>
+      <c r="D51" s="218"/>
       <c r="E51" s="135"/>
       <c r="F51" s="136"/>
       <c r="G51" s="124"/>
@@ -9591,14 +9591,14 @@
       <c r="F64" s="140"/>
     </row>
     <row r="66" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="217" t="s">
+      <c r="A66" s="227" t="s">
         <v>769</v>
       </c>
-      <c r="B66" s="217"/>
-      <c r="C66" s="217"/>
-      <c r="D66" s="217"/>
-      <c r="E66" s="217"/>
-      <c r="F66" s="217"/>
+      <c r="B66" s="227"/>
+      <c r="C66" s="227"/>
+      <c r="D66" s="227"/>
+      <c r="E66" s="227"/>
+      <c r="F66" s="227"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="95"/>
@@ -9610,7 +9610,7 @@
     </row>
     <row r="68" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A68" s="184" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -9744,10 +9744,10 @@
       </c>
       <c r="C78" s="50"/>
       <c r="D78" s="51"/>
-      <c r="E78" s="231" t="s">
+      <c r="E78" s="233" t="s">
         <v>94</v>
       </c>
-      <c r="F78" s="232"/>
+      <c r="F78" s="234"/>
     </row>
     <row r="79" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="46"/>
@@ -9866,10 +9866,10 @@
       <c r="B87" s="64"/>
       <c r="C87" s="64"/>
       <c r="D87" s="68"/>
-      <c r="E87" s="218" t="s">
+      <c r="E87" s="228" t="s">
         <v>119</v>
       </c>
-      <c r="F87" s="219"/>
+      <c r="F87" s="229"/>
     </row>
     <row r="88" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A88" s="69" t="s">
@@ -10098,10 +10098,10 @@
     <row r="101" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="46"/>
       <c r="B101" s="79"/>
-      <c r="C101" s="220" t="s">
+      <c r="C101" s="230" t="s">
         <v>180</v>
       </c>
-      <c r="D101" s="221"/>
+      <c r="D101" s="231"/>
       <c r="E101" s="80" t="s">
         <v>181</v>
       </c>
@@ -10118,8 +10118,8 @@
       <c r="D102" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="E102" s="229"/>
-      <c r="F102" s="230"/>
+      <c r="E102" s="215"/>
+      <c r="F102" s="216"/>
     </row>
     <row r="103" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="46"/>
@@ -10130,8 +10130,8 @@
       <c r="D103" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="E103" s="229"/>
-      <c r="F103" s="230"/>
+      <c r="E103" s="215"/>
+      <c r="F103" s="216"/>
     </row>
     <row r="104" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="46"/>
@@ -10142,8 +10142,8 @@
       <c r="D104" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="E104" s="229"/>
-      <c r="F104" s="230"/>
+      <c r="E104" s="215"/>
+      <c r="F104" s="216"/>
     </row>
     <row r="105" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="46"/>
@@ -10154,8 +10154,8 @@
       <c r="D105" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="E105" s="229"/>
-      <c r="F105" s="230"/>
+      <c r="E105" s="215"/>
+      <c r="F105" s="216"/>
     </row>
     <row r="106" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="46"/>
@@ -10166,8 +10166,8 @@
       <c r="D106" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="E106" s="229"/>
-      <c r="F106" s="230"/>
+      <c r="E106" s="215"/>
+      <c r="F106" s="216"/>
     </row>
     <row r="107" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="62"/>
@@ -10178,8 +10178,8 @@
       <c r="D107" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="E107" s="215"/>
-      <c r="F107" s="216"/>
+      <c r="E107" s="225"/>
+      <c r="F107" s="226"/>
     </row>
     <row r="108" spans="1:6" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="84" t="s">
@@ -10366,13 +10366,6 @@
     <row r="122" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E102:F102"/>
     <mergeCell ref="E107:F107"/>
     <mergeCell ref="A66:F66"/>
     <mergeCell ref="E87:F87"/>
@@ -10389,6 +10382,13 @@
     <mergeCell ref="E103:F103"/>
     <mergeCell ref="E104:F104"/>
     <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E102:F102"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.59" right="0.59" top="0.59" bottom="0.59" header="0.39000000000000007" footer="0.39000000000000007"/>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -10487,7 +10487,7 @@
         <v>751</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -10504,10 +10504,10 @@
         <v>266</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10624,7 +10624,7 @@
         <v>258</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>262</v>
@@ -10638,7 +10638,7 @@
         <v>260</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>263</v>
@@ -10648,7 +10648,7 @@
       <c r="A17" s="143"/>
       <c r="B17" s="18"/>
       <c r="C17" s="5" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>264</v>
@@ -10702,7 +10702,7 @@
       <c r="A23" s="143"/>
       <c r="B23" s="18"/>
       <c r="C23" s="236" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D23" s="237"/>
     </row>
@@ -10715,7 +10715,7 @@
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="144"/>
       <c r="B25" s="134" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C25" s="100" t="s">
         <v>44</v>
@@ -10759,57 +10759,57 @@
         <v>776</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="143"/>
       <c r="B30" s="18"/>
       <c r="C30" s="5" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="143"/>
       <c r="B31" s="18"/>
       <c r="C31" s="5" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="143"/>
       <c r="B32" s="18"/>
       <c r="C32" s="5" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="143"/>
       <c r="B33" s="18"/>
       <c r="C33" s="5" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="143"/>
       <c r="B34" s="18"/>
       <c r="C34" s="5" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -10861,13 +10861,13 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="144"/>
       <c r="B40" s="134" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="C40" s="100" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="100" t="s">
-        <v>754</v>
+        <v>573</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -10875,27 +10875,27 @@
       <c r="B41" s="18"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="177" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="143"/>
       <c r="B42" s="18"/>
       <c r="C42" s="112" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D42" s="176" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="177" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="143"/>
       <c r="B43" s="18"/>
       <c r="C43" s="112" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="D43" s="176" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -10908,7 +10908,7 @@
       <c r="A45" s="143"/>
       <c r="B45" s="18"/>
       <c r="C45" s="235" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D45" s="235"/>
     </row>
@@ -11023,7 +11023,7 @@
     </row>
     <row r="57" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A57" s="184" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -11285,13 +11285,13 @@
         <v>280</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>789</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="113" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -11299,7 +11299,7 @@
         <v>282</v>
       </c>
       <c r="B7" s="102" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C7" s="102"/>
       <c r="D7" s="151"/>
@@ -11309,13 +11309,13 @@
         <v>291</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>790</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
@@ -11367,7 +11367,7 @@
         <v>305</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E13" s="115"/>
       <c r="F13" s="115"/>
@@ -11379,7 +11379,7 @@
         <v>301</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E14" s="115"/>
       <c r="F14" s="115"/>
@@ -11391,7 +11391,7 @@
         <v>308</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E15" s="115"/>
       <c r="F15" s="115"/>
@@ -11423,7 +11423,7 @@
       <c r="B18" s="183"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="G18" s="111"/>
       <c r="H18" s="18"/>
@@ -11445,7 +11445,7 @@
         <v>311</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.2">
@@ -11455,7 +11455,7 @@
         <v>316</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -11465,7 +11465,7 @@
         <v>323</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -11509,12 +11509,12 @@
         <v>329</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="184" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -11945,6 +11945,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
     <mergeCell ref="H38:H39"/>
     <mergeCell ref="H40:H41"/>
     <mergeCell ref="A42:A43"/>
@@ -11960,18 +11972,6 @@
     <mergeCell ref="G40:G41"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.59" right="0.59" top="0.59" bottom="0.59" header="0.39000000000000007" footer="0.39000000000000007"/>
@@ -12051,13 +12051,13 @@
         <v>791</v>
       </c>
       <c r="B6" s="176" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C6" s="112" t="s">
         <v>793</v>
       </c>
       <c r="D6" s="176" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -12065,13 +12065,13 @@
         <v>337</v>
       </c>
       <c r="B7" s="176" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="C7" s="112" t="s">
         <v>794</v>
       </c>
       <c r="D7" s="176" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -12079,13 +12079,13 @@
         <v>338</v>
       </c>
       <c r="B8" s="176" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C8" s="112" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D8" s="176" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -12093,7 +12093,7 @@
         <v>339</v>
       </c>
       <c r="B9" s="176" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="C9" s="112"/>
       <c r="D9" s="176"/>
@@ -12854,7 +12854,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="B1" s="194"/>
       <c r="D1" s="194"/>
@@ -12897,7 +12897,7 @@
         <v>751</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="31" t="s">
@@ -13121,7 +13121,7 @@
     </row>
     <row r="27" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="242" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="B27" s="242"/>
       <c r="C27" s="242"/>
@@ -13181,13 +13181,13 @@
         <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -13215,13 +13215,13 @@
         <v>751</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>751</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -13258,18 +13258,18 @@
         <v>44</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="137"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="9" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -13299,7 +13299,7 @@
         <v>529</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -13395,18 +13395,18 @@
         <v>44</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="137"/>
       <c r="C20" s="10"/>
       <c r="D20" s="9" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -13436,7 +13436,7 @@
         <v>529</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix typo in home table and remove MR99 from Table2
</commit_message>
<xml_diff>
--- a/Taxonomy_tables_v3.2.xlsx
+++ b/Taxonomy_tables_v3.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cye/Documents/wip/gem_taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AD23FB-D539-4E4B-A7E8-B48676B0CE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15249079-317A-E947-8273-768DB67A5DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1460" yWindow="-19800" windowWidth="28800" windowHeight="17500" tabRatio="694" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taxonomy v3.2" sheetId="1" r:id="rId1"/>
@@ -2839,9 +2839,6 @@
     <t>Attribute 13</t>
   </si>
   <si>
-    <t>Dettached</t>
-  </si>
-  <si>
     <t>Rectangular</t>
   </si>
   <si>
@@ -3392,6 +3389,9 @@
   </si>
   <si>
     <t xml:space="preserve">    Lateral load coefficcient (Level 1.1)</t>
+  </si>
+  <si>
+    <t>Detached</t>
   </si>
 </sst>
 </file>
@@ -4625,7 +4625,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="252">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5334,6 +5334,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="77">
@@ -5825,7 +5828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -5846,7 +5849,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="199" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -5895,7 +5898,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="187" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F5" s="187" t="s">
         <v>10</v>
@@ -5916,7 +5919,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="187" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F6" s="203" t="s">
         <v>10</v>
@@ -5931,7 +5934,7 @@
       <c r="C7" s="203"/>
       <c r="D7" s="204"/>
       <c r="E7" s="187" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F7" s="203"/>
       <c r="G7" s="203"/>
@@ -5942,7 +5945,7 @@
       <c r="C8" s="203"/>
       <c r="D8" s="204"/>
       <c r="E8" s="187" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="F8" s="203"/>
       <c r="G8" s="203"/>
@@ -5953,7 +5956,7 @@
       <c r="C9" s="203"/>
       <c r="D9" s="204"/>
       <c r="E9" s="187" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F9" s="203"/>
       <c r="G9" s="203"/>
@@ -5970,7 +5973,7 @@
         <v>13</v>
       </c>
       <c r="E10" s="187" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F10" s="203" t="s">
         <v>10</v>
@@ -5985,7 +5988,7 @@
       <c r="C11" s="203"/>
       <c r="D11" s="204"/>
       <c r="E11" s="187" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="F11" s="203"/>
       <c r="G11" s="203"/>
@@ -5996,7 +5999,7 @@
       <c r="C12" s="203"/>
       <c r="D12" s="204"/>
       <c r="E12" s="187" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F12" s="203"/>
       <c r="G12" s="203"/>
@@ -6007,7 +6010,7 @@
       <c r="C13" s="203"/>
       <c r="D13" s="204"/>
       <c r="E13" s="187" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F13" s="203"/>
       <c r="G13" s="203"/>
@@ -6018,7 +6021,7 @@
       <c r="C14" s="203"/>
       <c r="D14" s="204"/>
       <c r="E14" s="187" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F14" s="203"/>
       <c r="G14" s="203"/>
@@ -6029,7 +6032,7 @@
       <c r="C15" s="203"/>
       <c r="D15" s="204"/>
       <c r="E15" s="187" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F15" s="203"/>
       <c r="G15" s="203"/>
@@ -6048,7 +6051,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="187" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F16" s="187" t="s">
         <v>19</v>
@@ -6063,10 +6066,10 @@
       <c r="C17" s="209"/>
       <c r="D17" s="212"/>
       <c r="E17" s="187" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F17" s="187" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G17" s="187">
         <v>22.6</v>
@@ -6078,7 +6081,7 @@
       <c r="C18" s="209"/>
       <c r="D18" s="212"/>
       <c r="E18" s="187" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F18" s="187" t="s">
         <v>19</v>
@@ -6093,10 +6096,10 @@
       <c r="C19" s="209"/>
       <c r="D19" s="212"/>
       <c r="E19" s="187" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F19" s="191" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G19" s="187">
         <v>0.5</v>
@@ -6108,10 +6111,10 @@
       <c r="C20" s="210"/>
       <c r="D20" s="213"/>
       <c r="E20" s="187" t="s">
+        <v>857</v>
+      </c>
+      <c r="F20" s="187" t="s">
         <v>858</v>
-      </c>
-      <c r="F20" s="187" t="s">
-        <v>859</v>
       </c>
       <c r="G20" s="187">
         <v>2</v>
@@ -6129,7 +6132,7 @@
         <v>23</v>
       </c>
       <c r="E21" s="187" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F21" s="187" t="s">
         <v>19</v>
@@ -6144,7 +6147,7 @@
       <c r="C22" s="210"/>
       <c r="D22" s="204"/>
       <c r="E22" s="187" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="F22" s="187" t="s">
         <v>10</v>
@@ -6163,7 +6166,7 @@
         <v>21</v>
       </c>
       <c r="E23" s="187" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="F23" s="203" t="s">
         <v>10</v>
@@ -6178,7 +6181,7 @@
       <c r="C24" s="203"/>
       <c r="D24" s="213"/>
       <c r="E24" s="187" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F24" s="203"/>
       <c r="G24" s="203"/>
@@ -6197,13 +6200,13 @@
         <v>26</v>
       </c>
       <c r="E25" s="187" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F25" s="187" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="187" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6212,13 +6215,13 @@
       <c r="C26" s="210"/>
       <c r="D26" s="213"/>
       <c r="E26" s="187" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F26" s="187" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="187" t="s">
-        <v>831</v>
+        <v>972</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -6233,7 +6236,7 @@
         <v>28</v>
       </c>
       <c r="E27" s="187" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F27" s="203" t="s">
         <v>10</v>
@@ -6248,7 +6251,7 @@
       <c r="C28" s="203"/>
       <c r="D28" s="212"/>
       <c r="E28" s="187" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F28" s="203"/>
       <c r="G28" s="203"/>
@@ -6259,7 +6262,7 @@
       <c r="C29" s="203"/>
       <c r="D29" s="212"/>
       <c r="E29" s="187" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F29" s="203"/>
       <c r="G29" s="203"/>
@@ -6270,7 +6273,7 @@
       <c r="C30" s="203"/>
       <c r="D30" s="212"/>
       <c r="E30" s="187" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F30" s="203"/>
       <c r="G30" s="203"/>
@@ -6281,7 +6284,7 @@
       <c r="C31" s="203"/>
       <c r="D31" s="213"/>
       <c r="E31" s="187" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F31" s="203"/>
       <c r="G31" s="203"/>
@@ -6298,7 +6301,7 @@
         <v>30</v>
       </c>
       <c r="E32" s="187" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F32" s="187" t="s">
         <v>10</v>
@@ -6320,7 +6323,7 @@
         <v>33</v>
       </c>
       <c r="E33" s="187" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F33" s="187" t="s">
         <v>10</v>
@@ -6336,7 +6339,7 @@
       <c r="C34" s="209"/>
       <c r="D34" s="212"/>
       <c r="E34" s="187" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F34" s="187" t="s">
         <v>10</v>
@@ -6352,7 +6355,7 @@
       <c r="C35" s="210"/>
       <c r="D35" s="213"/>
       <c r="E35" s="187" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="F35" s="187" t="s">
         <v>10</v>
@@ -6375,7 +6378,7 @@
         <v>39</v>
       </c>
       <c r="E36" s="187" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F36" s="203" t="s">
         <v>10</v>
@@ -6390,7 +6393,7 @@
       <c r="C37" s="203"/>
       <c r="D37" s="204"/>
       <c r="E37" s="187" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F37" s="203"/>
       <c r="G37" s="203"/>
@@ -6401,7 +6404,7 @@
       <c r="C38" s="203"/>
       <c r="D38" s="204"/>
       <c r="E38" s="187" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F38" s="203"/>
       <c r="G38" s="203"/>
@@ -6412,7 +6415,7 @@
       <c r="C39" s="203"/>
       <c r="D39" s="204"/>
       <c r="E39" s="187" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="F39" s="203"/>
       <c r="G39" s="203"/>
@@ -6423,7 +6426,7 @@
       <c r="C40" s="203"/>
       <c r="D40" s="204"/>
       <c r="E40" s="187" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F40" s="203"/>
       <c r="G40" s="203"/>
@@ -6440,7 +6443,7 @@
         <v>36</v>
       </c>
       <c r="E41" s="187" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F41" s="203" t="s">
         <v>10</v>
@@ -6455,7 +6458,7 @@
       <c r="C42" s="203"/>
       <c r="D42" s="204"/>
       <c r="E42" s="187" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F42" s="203"/>
       <c r="G42" s="187"/>
@@ -6466,7 +6469,7 @@
       <c r="C43" s="203"/>
       <c r="D43" s="204"/>
       <c r="E43" s="187" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="F43" s="203"/>
       <c r="G43" s="187"/>
@@ -6483,7 +6486,7 @@
         <v>42</v>
       </c>
       <c r="E44" s="187" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F44" s="187" t="s">
         <v>10</v>
@@ -6498,13 +6501,13 @@
         <v>14</v>
       </c>
       <c r="C45" s="187" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D45" s="189" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E45" s="187" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F45" s="187" t="s">
         <v>10</v>
@@ -6660,7 +6663,7 @@
         <v>809</v>
       </c>
       <c r="C5" s="244" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.2">
@@ -6668,7 +6671,7 @@
         <v>812</v>
       </c>
       <c r="B6" s="116" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C6" s="245"/>
     </row>
@@ -6677,7 +6680,7 @@
         <v>813</v>
       </c>
       <c r="B7" s="116" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C7" s="245"/>
     </row>
@@ -6686,7 +6689,7 @@
         <v>814</v>
       </c>
       <c r="B8" s="116" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C8" s="245"/>
     </row>
@@ -6695,7 +6698,7 @@
         <v>815</v>
       </c>
       <c r="B9" s="116" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C9" s="246"/>
     </row>
@@ -6995,7 +6998,7 @@
         <v>826</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>44</v>
@@ -7010,7 +7013,7 @@
         <v>542</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11" t="s">
@@ -7046,7 +7049,7 @@
         <v>816</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.2">
@@ -7063,7 +7066,7 @@
         <v>817</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.2">
@@ -7080,7 +7083,7 @@
         <v>818</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
@@ -7254,7 +7257,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>44</v>
@@ -7272,7 +7275,7 @@
         <v>44</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>44</v>
@@ -7328,7 +7331,7 @@
         <v>751</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.2">
@@ -7444,7 +7447,7 @@
         <v>612</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -7467,7 +7470,7 @@
         <v>622</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>627</v>
@@ -7632,13 +7635,13 @@
         <v>751</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>654</v>
       </c>
       <c r="H17" s="102" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="I17" s="143"/>
       <c r="J17" s="149"/>
@@ -7658,7 +7661,7 @@
         <v>655</v>
       </c>
       <c r="H18" s="102" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I18" s="249"/>
       <c r="J18" s="248"/>
@@ -7672,7 +7675,7 @@
         <v>656</v>
       </c>
       <c r="H19" s="102" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I19" s="249"/>
       <c r="J19" s="248"/>
@@ -7806,7 +7809,7 @@
         <v>672</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I27" s="143"/>
       <c r="J27" s="149"/>
@@ -7934,7 +7937,7 @@
         <v>44</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>44</v>
@@ -8386,7 +8389,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B1" s="16"/>
     </row>
@@ -8395,13 +8398,13 @@
         <v>44</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -8409,23 +8412,23 @@
         <v>751</v>
       </c>
       <c r="B5" s="119" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="119" t="s">
+        <v>836</v>
+      </c>
+      <c r="B6" s="119" t="s">
         <v>837</v>
-      </c>
-      <c r="B6" s="119" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="119" t="s">
+        <v>838</v>
+      </c>
+      <c r="B7" s="119" t="s">
         <v>839</v>
-      </c>
-      <c r="B7" s="119" t="s">
-        <v>840</v>
       </c>
     </row>
   </sheetData>
@@ -8548,7 +8551,7 @@
     </row>
     <row r="12" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="184" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -8676,8 +8679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C54" sqref="C54"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9167,7 +9170,7 @@
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="166"/>
       <c r="B32" s="167" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C32" s="170" t="s">
         <v>44</v>
@@ -9191,8 +9194,8 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="126"/>
       <c r="B34" s="127"/>
-      <c r="C34" s="122" t="s">
-        <v>183</v>
+      <c r="C34" s="251" t="s">
+        <v>751</v>
       </c>
       <c r="D34" s="101" t="s">
         <v>184</v>
@@ -9410,13 +9413,13 @@
     </row>
     <row r="51" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
+        <v>959</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>961</v>
+      </c>
+      <c r="C51" s="217" t="s">
         <v>960</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>962</v>
-      </c>
-      <c r="C51" s="217" t="s">
-        <v>961</v>
       </c>
       <c r="D51" s="218"/>
       <c r="E51" s="135"/>
@@ -9610,7 +9613,7 @@
     </row>
     <row r="68" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A68" s="184" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -10467,7 +10470,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -10487,7 +10490,7 @@
         <v>751</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
@@ -10504,10 +10507,10 @@
         <v>266</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>958</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -10624,7 +10627,7 @@
         <v>258</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>262</v>
@@ -10638,7 +10641,7 @@
         <v>260</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>263</v>
@@ -10648,7 +10651,7 @@
       <c r="A17" s="143"/>
       <c r="B17" s="18"/>
       <c r="C17" s="5" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>264</v>
@@ -10702,7 +10705,7 @@
       <c r="A23" s="143"/>
       <c r="B23" s="18"/>
       <c r="C23" s="236" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D23" s="237"/>
     </row>
@@ -10715,7 +10718,7 @@
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="144"/>
       <c r="B25" s="134" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C25" s="100" t="s">
         <v>44</v>
@@ -10759,57 +10762,57 @@
         <v>776</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="143"/>
       <c r="B30" s="18"/>
       <c r="C30" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>916</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="143"/>
       <c r="B31" s="18"/>
       <c r="C31" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>918</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="143"/>
       <c r="B32" s="18"/>
       <c r="C32" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>920</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="143"/>
       <c r="B33" s="18"/>
       <c r="C33" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>922</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="143"/>
       <c r="B34" s="18"/>
       <c r="C34" s="5" t="s">
+        <v>923</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>924</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -10861,7 +10864,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="144"/>
       <c r="B40" s="134" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C40" s="100" t="s">
         <v>44</v>
@@ -10875,27 +10878,27 @@
       <c r="B41" s="18"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="177" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="143"/>
       <c r="B42" s="18"/>
       <c r="C42" s="112" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D42" s="176" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="177" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="143"/>
       <c r="B43" s="18"/>
       <c r="C43" s="112" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D43" s="176" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -10908,7 +10911,7 @@
       <c r="A45" s="143"/>
       <c r="B45" s="18"/>
       <c r="C45" s="235" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="D45" s="235"/>
     </row>
@@ -11023,7 +11026,7 @@
     </row>
     <row r="57" spans="1:6" ht="21" x14ac:dyDescent="0.2">
       <c r="A57" s="184" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -11285,13 +11288,13 @@
         <v>280</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>789</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="113" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -11299,7 +11302,7 @@
         <v>282</v>
       </c>
       <c r="B7" s="102" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C7" s="102"/>
       <c r="D7" s="151"/>
@@ -11309,13 +11312,13 @@
         <v>291</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>790</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="113" customFormat="1" ht="14" x14ac:dyDescent="0.2">
@@ -11367,7 +11370,7 @@
         <v>305</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E13" s="115"/>
       <c r="F13" s="115"/>
@@ -11379,7 +11382,7 @@
         <v>301</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E14" s="115"/>
       <c r="F14" s="115"/>
@@ -11391,7 +11394,7 @@
         <v>308</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E15" s="115"/>
       <c r="F15" s="115"/>
@@ -11423,7 +11426,7 @@
       <c r="B18" s="183"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="G18" s="111"/>
       <c r="H18" s="18"/>
@@ -11445,7 +11448,7 @@
         <v>311</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.2">
@@ -11455,7 +11458,7 @@
         <v>316</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -11465,7 +11468,7 @@
         <v>323</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -11509,12 +11512,12 @@
         <v>329</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A30" s="184" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -11945,6 +11948,7 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A38:A39"/>
     <mergeCell ref="G47:G48"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="B54:B55"/>
@@ -11955,23 +11959,22 @@
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
     <mergeCell ref="H42:H43"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="E40:E41"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
     <mergeCell ref="B38:B39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H41"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.59" right="0.59" top="0.59" bottom="0.59" header="0.39000000000000007" footer="0.39000000000000007"/>
@@ -12051,13 +12054,13 @@
         <v>791</v>
       </c>
       <c r="B6" s="176" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C6" s="112" t="s">
         <v>793</v>
       </c>
       <c r="D6" s="176" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -12065,13 +12068,13 @@
         <v>337</v>
       </c>
       <c r="B7" s="176" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C7" s="112" t="s">
         <v>794</v>
       </c>
       <c r="D7" s="176" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -12079,13 +12082,13 @@
         <v>338</v>
       </c>
       <c r="B8" s="176" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C8" s="112" t="s">
+        <v>943</v>
+      </c>
+      <c r="D8" s="176" t="s">
         <v>944</v>
-      </c>
-      <c r="D8" s="176" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -12093,7 +12096,7 @@
         <v>339</v>
       </c>
       <c r="B9" s="176" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C9" s="112"/>
       <c r="D9" s="176"/>
@@ -12807,7 +12810,7 @@
     </row>
     <row r="59" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="241" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B59" s="241"/>
       <c r="C59" s="241"/>
@@ -12854,7 +12857,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B1" s="194"/>
       <c r="D1" s="194"/>
@@ -12897,7 +12900,7 @@
         <v>751</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="31" t="s">
@@ -13121,7 +13124,7 @@
     </row>
     <row r="27" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="242" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B27" s="242"/>
       <c r="C27" s="242"/>
@@ -13181,13 +13184,13 @@
         <v>44</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -13215,13 +13218,13 @@
         <v>751</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>751</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -13258,18 +13261,18 @@
         <v>44</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="137"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="9" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -13299,7 +13302,7 @@
         <v>529</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -13395,18 +13398,18 @@
         <v>44</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="137"/>
       <c r="C20" s="10"/>
       <c r="D20" s="9" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -13436,7 +13439,7 @@
         <v>529</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix taxonomy string for EDU2 in Taxonomy_tables_v3.2.xlsx, Table 6
</commit_message>
<xml_diff>
--- a/Taxonomy_tables_v3.2.xlsx
+++ b/Taxonomy_tables_v3.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cye/Documents/wip/gem_taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15249079-317A-E947-8273-768DB67A5DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B3635D-1A55-874D-8A53-DCD950C60668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="-19800" windowWidth="28800" windowHeight="17500" tabRatio="694" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="694" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taxonomy v3.2" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="974">
   <si>
     <t>#</t>
   </si>
@@ -3392,6 +3392,9 @@
   </si>
   <si>
     <t>Detached</t>
+  </si>
+  <si>
+    <t>EDU2</t>
   </si>
 </sst>
 </file>
@@ -5182,55 +5185,106 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5239,54 +5293,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5294,14 +5300,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5334,9 +5340,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="69" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="77">
@@ -5481,12 +5484,12 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38097" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -5853,39 +5856,39 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="213" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="201" t="s">
+      <c r="B3" s="214" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="200" t="s">
+      <c r="C3" s="213" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="200" t="s">
+      <c r="D3" s="213" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="200" t="s">
+      <c r="E3" s="213" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="200" t="s">
+      <c r="F3" s="213" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="200" t="s">
+      <c r="G3" s="213" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="200"/>
-      <c r="B4" s="201"/>
-      <c r="C4" s="200"/>
-      <c r="D4" s="200"/>
-      <c r="E4" s="200"/>
-      <c r="F4" s="200"/>
-      <c r="G4" s="200"/>
+      <c r="A4" s="213"/>
+      <c r="B4" s="214"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
     </row>
     <row r="5" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="203" t="s">
+      <c r="A5" s="205" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="188">
@@ -5908,146 +5911,146 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="203"/>
-      <c r="B6" s="202">
+      <c r="A6" s="205"/>
+      <c r="B6" s="204">
         <v>2</v>
       </c>
-      <c r="C6" s="203" t="s">
+      <c r="C6" s="205" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="204" t="s">
+      <c r="D6" s="206" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="187" t="s">
         <v>849</v>
       </c>
-      <c r="F6" s="203" t="s">
+      <c r="F6" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="203" t="s">
+      <c r="G6" s="205" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="203"/>
-      <c r="B7" s="202"/>
-      <c r="C7" s="203"/>
-      <c r="D7" s="204"/>
+      <c r="A7" s="205"/>
+      <c r="B7" s="204"/>
+      <c r="C7" s="205"/>
+      <c r="D7" s="206"/>
       <c r="E7" s="187" t="s">
         <v>845</v>
       </c>
-      <c r="F7" s="203"/>
-      <c r="G7" s="203"/>
+      <c r="F7" s="205"/>
+      <c r="G7" s="205"/>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="203"/>
-      <c r="B8" s="202"/>
-      <c r="C8" s="203"/>
-      <c r="D8" s="204"/>
+      <c r="A8" s="205"/>
+      <c r="B8" s="204"/>
+      <c r="C8" s="205"/>
+      <c r="D8" s="206"/>
       <c r="E8" s="187" t="s">
         <v>875</v>
       </c>
-      <c r="F8" s="203"/>
-      <c r="G8" s="203"/>
+      <c r="F8" s="205"/>
+      <c r="G8" s="205"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="203"/>
-      <c r="B9" s="202"/>
-      <c r="C9" s="203"/>
-      <c r="D9" s="204"/>
+      <c r="A9" s="205"/>
+      <c r="B9" s="204"/>
+      <c r="C9" s="205"/>
+      <c r="D9" s="206"/>
       <c r="E9" s="187" t="s">
         <v>847</v>
       </c>
-      <c r="F9" s="203"/>
-      <c r="G9" s="203"/>
+      <c r="F9" s="205"/>
+      <c r="G9" s="205"/>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="203"/>
-      <c r="B10" s="202">
+      <c r="A10" s="205"/>
+      <c r="B10" s="204">
         <v>3</v>
       </c>
-      <c r="C10" s="203" t="s">
+      <c r="C10" s="205" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="204" t="s">
+      <c r="D10" s="206" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="187" t="s">
         <v>850</v>
       </c>
-      <c r="F10" s="203" t="s">
+      <c r="F10" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="203" t="s">
+      <c r="G10" s="205" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="203"/>
-      <c r="B11" s="202"/>
-      <c r="C11" s="203"/>
-      <c r="D11" s="204"/>
+      <c r="A11" s="205"/>
+      <c r="B11" s="204"/>
+      <c r="C11" s="205"/>
+      <c r="D11" s="206"/>
       <c r="E11" s="187" t="s">
         <v>969</v>
       </c>
-      <c r="F11" s="203"/>
-      <c r="G11" s="203"/>
+      <c r="F11" s="205"/>
+      <c r="G11" s="205"/>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="203"/>
-      <c r="B12" s="202"/>
-      <c r="C12" s="203"/>
-      <c r="D12" s="204"/>
+      <c r="A12" s="205"/>
+      <c r="B12" s="204"/>
+      <c r="C12" s="205"/>
+      <c r="D12" s="206"/>
       <c r="E12" s="187" t="s">
         <v>971</v>
       </c>
-      <c r="F12" s="203"/>
-      <c r="G12" s="203"/>
+      <c r="F12" s="205"/>
+      <c r="G12" s="205"/>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="203"/>
-      <c r="B13" s="202"/>
-      <c r="C13" s="203"/>
-      <c r="D13" s="204"/>
+      <c r="A13" s="205"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="205"/>
+      <c r="D13" s="206"/>
       <c r="E13" s="187" t="s">
         <v>970</v>
       </c>
-      <c r="F13" s="203"/>
-      <c r="G13" s="203"/>
+      <c r="F13" s="205"/>
+      <c r="G13" s="205"/>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="203"/>
-      <c r="B14" s="202"/>
-      <c r="C14" s="203"/>
-      <c r="D14" s="204"/>
+      <c r="A14" s="205"/>
+      <c r="B14" s="204"/>
+      <c r="C14" s="205"/>
+      <c r="D14" s="206"/>
       <c r="E14" s="187" t="s">
         <v>851</v>
       </c>
-      <c r="F14" s="203"/>
-      <c r="G14" s="203"/>
+      <c r="F14" s="205"/>
+      <c r="G14" s="205"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="203"/>
-      <c r="B15" s="202"/>
-      <c r="C15" s="203"/>
-      <c r="D15" s="204"/>
+      <c r="A15" s="205"/>
+      <c r="B15" s="204"/>
+      <c r="C15" s="205"/>
+      <c r="D15" s="206"/>
       <c r="E15" s="187" t="s">
         <v>852</v>
       </c>
-      <c r="F15" s="203"/>
-      <c r="G15" s="203"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="203" t="s">
+      <c r="A16" s="205" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="205">
+      <c r="B16" s="209">
         <v>4</v>
       </c>
-      <c r="C16" s="208" t="s">
+      <c r="C16" s="201" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="211" t="s">
+      <c r="D16" s="207" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="187" t="s">
@@ -6061,10 +6064,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="203"/>
-      <c r="B17" s="206"/>
-      <c r="C17" s="209"/>
-      <c r="D17" s="212"/>
+      <c r="A17" s="205"/>
+      <c r="B17" s="212"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="211"/>
       <c r="E17" s="187" t="s">
         <v>854</v>
       </c>
@@ -6076,10 +6079,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="203"/>
-      <c r="B18" s="206"/>
-      <c r="C18" s="209"/>
-      <c r="D18" s="212"/>
+      <c r="A18" s="205"/>
+      <c r="B18" s="212"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="211"/>
       <c r="E18" s="187" t="s">
         <v>855</v>
       </c>
@@ -6091,10 +6094,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="203"/>
-      <c r="B19" s="206"/>
-      <c r="C19" s="209"/>
-      <c r="D19" s="212"/>
+      <c r="A19" s="205"/>
+      <c r="B19" s="212"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="211"/>
       <c r="E19" s="187" t="s">
         <v>856</v>
       </c>
@@ -6106,10 +6109,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="203"/>
-      <c r="B20" s="207"/>
-      <c r="C20" s="210"/>
-      <c r="D20" s="213"/>
+      <c r="A20" s="205"/>
+      <c r="B20" s="210"/>
+      <c r="C20" s="203"/>
+      <c r="D20" s="208"/>
       <c r="E20" s="187" t="s">
         <v>857</v>
       </c>
@@ -6121,14 +6124,14 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="203"/>
-      <c r="B21" s="205">
+      <c r="A21" s="205"/>
+      <c r="B21" s="209">
         <v>5</v>
       </c>
-      <c r="C21" s="208" t="s">
+      <c r="C21" s="201" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="204" t="s">
+      <c r="D21" s="206" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="187" t="s">
@@ -6142,10 +6145,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="207"/>
-      <c r="C22" s="210"/>
-      <c r="D22" s="204"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="210"/>
+      <c r="C22" s="203"/>
+      <c r="D22" s="206"/>
       <c r="E22" s="187" t="s">
         <v>864</v>
       </c>
@@ -6155,48 +6158,48 @@
       <c r="G22" s="187"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="203"/>
-      <c r="B23" s="202">
+      <c r="A23" s="205"/>
+      <c r="B23" s="204">
         <v>6</v>
       </c>
-      <c r="C23" s="203" t="s">
+      <c r="C23" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="211" t="s">
+      <c r="D23" s="207" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="187" t="s">
         <v>865</v>
       </c>
-      <c r="F23" s="203" t="s">
+      <c r="F23" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="203" t="s">
+      <c r="G23" s="205" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="203"/>
-      <c r="B24" s="202"/>
-      <c r="C24" s="203"/>
-      <c r="D24" s="213"/>
+      <c r="A24" s="205"/>
+      <c r="B24" s="204"/>
+      <c r="C24" s="205"/>
+      <c r="D24" s="208"/>
       <c r="E24" s="187" t="s">
         <v>848</v>
       </c>
-      <c r="F24" s="203"/>
-      <c r="G24" s="203"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="203" t="s">
+      <c r="A25" s="205" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="205">
+      <c r="B25" s="209">
         <v>7</v>
       </c>
-      <c r="C25" s="208" t="s">
+      <c r="C25" s="201" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="211" t="s">
+      <c r="D25" s="207" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="187" t="s">
@@ -6210,10 +6213,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="203"/>
-      <c r="B26" s="207"/>
-      <c r="C26" s="210"/>
-      <c r="D26" s="213"/>
+      <c r="A26" s="205"/>
+      <c r="B26" s="210"/>
+      <c r="C26" s="203"/>
+      <c r="D26" s="208"/>
       <c r="E26" s="187" t="s">
         <v>867</v>
       </c>
@@ -6225,72 +6228,72 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="203"/>
-      <c r="B27" s="202">
+      <c r="A27" s="205"/>
+      <c r="B27" s="204">
         <v>8</v>
       </c>
-      <c r="C27" s="203" t="s">
+      <c r="C27" s="205" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="211" t="s">
+      <c r="D27" s="207" t="s">
         <v>28</v>
       </c>
       <c r="E27" s="187" t="s">
         <v>868</v>
       </c>
-      <c r="F27" s="203" t="s">
+      <c r="F27" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="203" t="s">
+      <c r="G27" s="205" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="203"/>
-      <c r="B28" s="202"/>
-      <c r="C28" s="203"/>
-      <c r="D28" s="212"/>
+      <c r="A28" s="205"/>
+      <c r="B28" s="204"/>
+      <c r="C28" s="205"/>
+      <c r="D28" s="211"/>
       <c r="E28" s="187" t="s">
         <v>872</v>
       </c>
-      <c r="F28" s="203"/>
-      <c r="G28" s="203"/>
+      <c r="F28" s="205"/>
+      <c r="G28" s="205"/>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="203"/>
-      <c r="B29" s="202"/>
-      <c r="C29" s="203"/>
-      <c r="D29" s="212"/>
+      <c r="A29" s="205"/>
+      <c r="B29" s="204"/>
+      <c r="C29" s="205"/>
+      <c r="D29" s="211"/>
       <c r="E29" s="187" t="s">
         <v>873</v>
       </c>
-      <c r="F29" s="203"/>
-      <c r="G29" s="203"/>
+      <c r="F29" s="205"/>
+      <c r="G29" s="205"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="203"/>
-      <c r="B30" s="202"/>
-      <c r="C30" s="203"/>
-      <c r="D30" s="212"/>
+      <c r="A30" s="205"/>
+      <c r="B30" s="204"/>
+      <c r="C30" s="205"/>
+      <c r="D30" s="211"/>
       <c r="E30" s="187" t="s">
         <v>869</v>
       </c>
-      <c r="F30" s="203"/>
-      <c r="G30" s="203"/>
+      <c r="F30" s="205"/>
+      <c r="G30" s="205"/>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A31" s="203"/>
-      <c r="B31" s="202"/>
-      <c r="C31" s="203"/>
-      <c r="D31" s="213"/>
+      <c r="A31" s="205"/>
+      <c r="B31" s="204"/>
+      <c r="C31" s="205"/>
+      <c r="D31" s="208"/>
       <c r="E31" s="187" t="s">
         <v>874</v>
       </c>
-      <c r="F31" s="203"/>
-      <c r="G31" s="203"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="203"/>
+      <c r="A32" s="205"/>
       <c r="B32" s="188">
         <v>9</v>
       </c>
@@ -6312,14 +6315,14 @@
       <c r="I32" s="193"/>
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="203"/>
-      <c r="B33" s="205">
+      <c r="A33" s="205"/>
+      <c r="B33" s="209">
         <v>10</v>
       </c>
-      <c r="C33" s="208" t="s">
+      <c r="C33" s="201" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="211" t="s">
+      <c r="D33" s="207" t="s">
         <v>33</v>
       </c>
       <c r="E33" s="187" t="s">
@@ -6334,10 +6337,10 @@
       <c r="I33" s="193"/>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="203"/>
-      <c r="B34" s="206"/>
-      <c r="C34" s="209"/>
-      <c r="D34" s="212"/>
+      <c r="A34" s="205"/>
+      <c r="B34" s="212"/>
+      <c r="C34" s="202"/>
+      <c r="D34" s="211"/>
       <c r="E34" s="187" t="s">
         <v>884</v>
       </c>
@@ -6350,10 +6353,10 @@
       <c r="I34" s="193"/>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="203"/>
-      <c r="B35" s="207"/>
-      <c r="C35" s="210"/>
-      <c r="D35" s="213"/>
+      <c r="A35" s="205"/>
+      <c r="B35" s="210"/>
+      <c r="C35" s="203"/>
+      <c r="D35" s="208"/>
       <c r="E35" s="187" t="s">
         <v>885</v>
       </c>
@@ -6365,87 +6368,87 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="208" t="s">
+      <c r="A36" s="201" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="202">
+      <c r="B36" s="204">
         <v>11</v>
       </c>
-      <c r="C36" s="203" t="s">
+      <c r="C36" s="205" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="204" t="s">
+      <c r="D36" s="206" t="s">
         <v>39</v>
       </c>
       <c r="E36" s="187" t="s">
         <v>877</v>
       </c>
-      <c r="F36" s="203" t="s">
+      <c r="F36" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="203" t="s">
+      <c r="G36" s="205" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="209"/>
-      <c r="B37" s="202"/>
-      <c r="C37" s="203"/>
-      <c r="D37" s="204"/>
+      <c r="A37" s="202"/>
+      <c r="B37" s="204"/>
+      <c r="C37" s="205"/>
+      <c r="D37" s="206"/>
       <c r="E37" s="187" t="s">
         <v>878</v>
       </c>
-      <c r="F37" s="203"/>
-      <c r="G37" s="203"/>
+      <c r="F37" s="205"/>
+      <c r="G37" s="205"/>
     </row>
     <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="209"/>
-      <c r="B38" s="202"/>
-      <c r="C38" s="203"/>
-      <c r="D38" s="204"/>
+      <c r="A38" s="202"/>
+      <c r="B38" s="204"/>
+      <c r="C38" s="205"/>
+      <c r="D38" s="206"/>
       <c r="E38" s="187" t="s">
         <v>879</v>
       </c>
-      <c r="F38" s="203"/>
-      <c r="G38" s="203"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
     </row>
     <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="209"/>
-      <c r="B39" s="202"/>
-      <c r="C39" s="203"/>
-      <c r="D39" s="204"/>
+      <c r="A39" s="202"/>
+      <c r="B39" s="204"/>
+      <c r="C39" s="205"/>
+      <c r="D39" s="206"/>
       <c r="E39" s="187" t="s">
         <v>880</v>
       </c>
-      <c r="F39" s="203"/>
-      <c r="G39" s="203"/>
+      <c r="F39" s="205"/>
+      <c r="G39" s="205"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="209"/>
-      <c r="B40" s="202"/>
-      <c r="C40" s="203"/>
-      <c r="D40" s="204"/>
+      <c r="A40" s="202"/>
+      <c r="B40" s="204"/>
+      <c r="C40" s="205"/>
+      <c r="D40" s="206"/>
       <c r="E40" s="187" t="s">
         <v>881</v>
       </c>
-      <c r="F40" s="203"/>
-      <c r="G40" s="203"/>
+      <c r="F40" s="205"/>
+      <c r="G40" s="205"/>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="209"/>
-      <c r="B41" s="202">
+      <c r="A41" s="202"/>
+      <c r="B41" s="204">
         <v>12</v>
       </c>
-      <c r="C41" s="203" t="s">
+      <c r="C41" s="205" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="204" t="s">
+      <c r="D41" s="206" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="187" t="s">
         <v>861</v>
       </c>
-      <c r="F41" s="203" t="s">
+      <c r="F41" s="205" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="187" t="s">
@@ -6453,29 +6456,29 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="209"/>
-      <c r="B42" s="202"/>
-      <c r="C42" s="203"/>
-      <c r="D42" s="204"/>
+      <c r="A42" s="202"/>
+      <c r="B42" s="204"/>
+      <c r="C42" s="205"/>
+      <c r="D42" s="206"/>
       <c r="E42" s="187" t="s">
         <v>862</v>
       </c>
-      <c r="F42" s="203"/>
+      <c r="F42" s="205"/>
       <c r="G42" s="187"/>
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="209"/>
-      <c r="B43" s="202"/>
-      <c r="C43" s="203"/>
-      <c r="D43" s="204"/>
+      <c r="A43" s="202"/>
+      <c r="B43" s="204"/>
+      <c r="C43" s="205"/>
+      <c r="D43" s="206"/>
       <c r="E43" s="187" t="s">
         <v>876</v>
       </c>
-      <c r="F43" s="203"/>
+      <c r="F43" s="205"/>
       <c r="G43" s="187"/>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="209"/>
+      <c r="A44" s="202"/>
       <c r="B44" s="188">
         <v>13</v>
       </c>
@@ -6496,7 +6499,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="210"/>
+      <c r="A45" s="203"/>
       <c r="B45" s="188">
         <v>14</v>
       </c>
@@ -6516,31 +6519,18 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="A25:A35"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="G36:G40"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="F10:F15"/>
     <mergeCell ref="G10:G15"/>
     <mergeCell ref="A16:A24"/>
@@ -6556,18 +6546,31 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G27:G31"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="G36:G40"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A36:A45"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A25:A35"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
@@ -6662,7 +6665,7 @@
       <c r="B5" s="116" t="s">
         <v>809</v>
       </c>
-      <c r="C5" s="244" t="s">
+      <c r="C5" s="245" t="s">
         <v>950</v>
       </c>
     </row>
@@ -6673,7 +6676,7 @@
       <c r="B6" s="116" t="s">
         <v>947</v>
       </c>
-      <c r="C6" s="245"/>
+      <c r="C6" s="246"/>
     </row>
     <row r="7" spans="1:6" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="116" t="s">
@@ -6682,7 +6685,7 @@
       <c r="B7" s="116" t="s">
         <v>948</v>
       </c>
-      <c r="C7" s="245"/>
+      <c r="C7" s="246"/>
     </row>
     <row r="8" spans="1:6" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="116" t="s">
@@ -6691,7 +6694,7 @@
       <c r="B8" s="116" t="s">
         <v>949</v>
       </c>
-      <c r="C8" s="245"/>
+      <c r="C8" s="246"/>
     </row>
     <row r="9" spans="1:6" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="116" t="s">
@@ -6700,7 +6703,7 @@
       <c r="B9" s="116" t="s">
         <v>949</v>
       </c>
-      <c r="C9" s="246"/>
+      <c r="C9" s="247"/>
     </row>
     <row r="10" spans="1:6" s="117" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A10" s="118"/>
@@ -7647,8 +7650,8 @@
       <c r="J17" s="149"/>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="A18" s="249"/>
-      <c r="B18" s="242"/>
+      <c r="A18" s="250"/>
+      <c r="B18" s="243"/>
       <c r="C18" s="5" t="s">
         <v>648</v>
       </c>
@@ -7663,12 +7666,12 @@
       <c r="H18" s="102" t="s">
         <v>908</v>
       </c>
-      <c r="I18" s="249"/>
-      <c r="J18" s="248"/>
+      <c r="I18" s="250"/>
+      <c r="J18" s="249"/>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="249"/>
-      <c r="B19" s="242"/>
+      <c r="A19" s="250"/>
+      <c r="B19" s="243"/>
       <c r="E19" s="143"/>
       <c r="F19" s="149"/>
       <c r="G19" s="5" t="s">
@@ -7677,8 +7680,8 @@
       <c r="H19" s="102" t="s">
         <v>909</v>
       </c>
-      <c r="I19" s="249"/>
-      <c r="J19" s="248"/>
+      <c r="I19" s="250"/>
+      <c r="J19" s="249"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="143"/>
@@ -7867,18 +7870,18 @@
       <c r="J30" s="154"/>
     </row>
     <row r="32" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="247" t="s">
+      <c r="A32" s="248" t="s">
         <v>739</v>
       </c>
-      <c r="B32" s="247"/>
-      <c r="C32" s="247"/>
-      <c r="D32" s="247"/>
-      <c r="E32" s="247"/>
-      <c r="F32" s="247"/>
-      <c r="G32" s="247"/>
-      <c r="H32" s="247"/>
-      <c r="I32" s="247"/>
-      <c r="J32" s="247"/>
+      <c r="B32" s="248"/>
+      <c r="C32" s="248"/>
+      <c r="D32" s="248"/>
+      <c r="E32" s="248"/>
+      <c r="F32" s="248"/>
+      <c r="G32" s="248"/>
+      <c r="H32" s="248"/>
+      <c r="I32" s="248"/>
+      <c r="J32" s="248"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8011,10 +8014,10 @@
       <c r="D7" s="5" t="s">
         <v>599</v>
       </c>
-      <c r="E7" s="250" t="s">
+      <c r="E7" s="251" t="s">
         <v>691</v>
       </c>
-      <c r="F7" s="250" t="s">
+      <c r="F7" s="251" t="s">
         <v>692</v>
       </c>
     </row>
@@ -8027,8 +8030,8 @@
       <c r="D8" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="E8" s="250"/>
-      <c r="F8" s="250"/>
+      <c r="E8" s="251"/>
+      <c r="F8" s="251"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="143"/>
@@ -8039,8 +8042,8 @@
       <c r="D9" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="E9" s="250"/>
-      <c r="F9" s="250"/>
+      <c r="E9" s="251"/>
+      <c r="F9" s="251"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="145"/>
@@ -8051,8 +8054,8 @@
       <c r="D10" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="E10" s="250"/>
-      <c r="F10" s="250"/>
+      <c r="E10" s="251"/>
+      <c r="F10" s="251"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
@@ -8349,10 +8352,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="242" t="s">
+      <c r="A12" s="243" t="s">
         <v>736</v>
       </c>
-      <c r="B12" s="242"/>
+      <c r="B12" s="243"/>
       <c r="C12" s="115"/>
     </row>
   </sheetData>
@@ -8532,11 +8535,11 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="214" t="s">
+      <c r="A10" s="215" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="214"/>
-      <c r="C10" s="214"/>
+      <c r="B10" s="215"/>
+      <c r="C10" s="215"/>
       <c r="D10" s="103"/>
       <c r="E10" s="103"/>
       <c r="F10" s="103"/>
@@ -8679,7 +8682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C54" sqref="C54"/>
       <selection pane="bottomLeft"/>
@@ -8744,8 +8747,8 @@
       </c>
       <c r="C5" s="102"/>
       <c r="D5" s="151"/>
-      <c r="E5" s="232"/>
-      <c r="F5" s="220"/>
+      <c r="E5" s="223"/>
+      <c r="F5" s="224"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -8760,8 +8763,8 @@
       <c r="D6" s="174" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="219"/>
-      <c r="F6" s="220"/>
+      <c r="E6" s="225"/>
+      <c r="F6" s="224"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -8776,8 +8779,8 @@
       <c r="D7" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="221"/>
-      <c r="F7" s="222"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="227"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -8792,8 +8795,8 @@
       <c r="D8" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="221"/>
-      <c r="F8" s="222"/>
+      <c r="E8" s="226"/>
+      <c r="F8" s="227"/>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
@@ -8808,8 +8811,8 @@
       <c r="D9" s="102" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="221"/>
-      <c r="F9" s="222"/>
+      <c r="E9" s="226"/>
+      <c r="F9" s="227"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="120"/>
@@ -8820,8 +8823,8 @@
       <c r="D10" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="223"/>
-      <c r="F10" s="224"/>
+      <c r="E10" s="228"/>
+      <c r="F10" s="229"/>
     </row>
     <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
@@ -8844,8 +8847,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="219"/>
-      <c r="B12" s="220"/>
+      <c r="A12" s="225"/>
+      <c r="B12" s="224"/>
       <c r="C12" s="151" t="s">
         <v>99</v>
       </c>
@@ -8860,8 +8863,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="221"/>
-      <c r="B13" s="222"/>
+      <c r="A13" s="226"/>
+      <c r="B13" s="227"/>
       <c r="C13" s="151" t="s">
         <v>103</v>
       </c>
@@ -8876,8 +8879,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="223"/>
-      <c r="B14" s="224"/>
+      <c r="A14" s="228"/>
+      <c r="B14" s="229"/>
       <c r="C14" s="151" t="s">
         <v>107</v>
       </c>
@@ -8904,8 +8907,8 @@
       <c r="D15" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="E15" s="219"/>
-      <c r="F15" s="220"/>
+      <c r="E15" s="225"/>
+      <c r="F15" s="224"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="163"/>
@@ -8916,8 +8919,8 @@
       <c r="D16" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="E16" s="221"/>
-      <c r="F16" s="222"/>
+      <c r="E16" s="226"/>
+      <c r="F16" s="227"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="164"/>
@@ -8928,8 +8931,8 @@
       <c r="D17" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="223"/>
-      <c r="F17" s="224"/>
+      <c r="E17" s="228"/>
+      <c r="F17" s="229"/>
     </row>
     <row r="18" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
@@ -9194,7 +9197,7 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="126"/>
       <c r="B34" s="127"/>
-      <c r="C34" s="251" t="s">
+      <c r="C34" s="200" t="s">
         <v>751</v>
       </c>
       <c r="D34" s="101" t="s">
@@ -9418,10 +9421,10 @@
       <c r="B51" s="19" t="s">
         <v>961</v>
       </c>
-      <c r="C51" s="217" t="s">
+      <c r="C51" s="234" t="s">
         <v>960</v>
       </c>
-      <c r="D51" s="218"/>
+      <c r="D51" s="235"/>
       <c r="E51" s="135"/>
       <c r="F51" s="136"/>
       <c r="G51" s="124"/>
@@ -9594,14 +9597,14 @@
       <c r="F64" s="140"/>
     </row>
     <row r="66" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="227" t="s">
+      <c r="A66" s="218" t="s">
         <v>769</v>
       </c>
-      <c r="B66" s="227"/>
-      <c r="C66" s="227"/>
-      <c r="D66" s="227"/>
-      <c r="E66" s="227"/>
-      <c r="F66" s="227"/>
+      <c r="B66" s="218"/>
+      <c r="C66" s="218"/>
+      <c r="D66" s="218"/>
+      <c r="E66" s="218"/>
+      <c r="F66" s="218"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="95"/>
@@ -9747,10 +9750,10 @@
       </c>
       <c r="C78" s="50"/>
       <c r="D78" s="51"/>
-      <c r="E78" s="233" t="s">
+      <c r="E78" s="232" t="s">
         <v>94</v>
       </c>
-      <c r="F78" s="234"/>
+      <c r="F78" s="233"/>
     </row>
     <row r="79" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="46"/>
@@ -9869,10 +9872,10 @@
       <c r="B87" s="64"/>
       <c r="C87" s="64"/>
       <c r="D87" s="68"/>
-      <c r="E87" s="228" t="s">
+      <c r="E87" s="219" t="s">
         <v>119</v>
       </c>
-      <c r="F87" s="229"/>
+      <c r="F87" s="220"/>
     </row>
     <row r="88" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A88" s="69" t="s">
@@ -10101,10 +10104,10 @@
     <row r="101" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="46"/>
       <c r="B101" s="79"/>
-      <c r="C101" s="230" t="s">
+      <c r="C101" s="221" t="s">
         <v>180</v>
       </c>
-      <c r="D101" s="231"/>
+      <c r="D101" s="222"/>
       <c r="E101" s="80" t="s">
         <v>181</v>
       </c>
@@ -10121,8 +10124,8 @@
       <c r="D102" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="E102" s="215"/>
-      <c r="F102" s="216"/>
+      <c r="E102" s="230"/>
+      <c r="F102" s="231"/>
     </row>
     <row r="103" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="46"/>
@@ -10133,8 +10136,8 @@
       <c r="D103" s="82" t="s">
         <v>186</v>
       </c>
-      <c r="E103" s="215"/>
-      <c r="F103" s="216"/>
+      <c r="E103" s="230"/>
+      <c r="F103" s="231"/>
     </row>
     <row r="104" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A104" s="46"/>
@@ -10145,8 +10148,8 @@
       <c r="D104" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="E104" s="215"/>
-      <c r="F104" s="216"/>
+      <c r="E104" s="230"/>
+      <c r="F104" s="231"/>
     </row>
     <row r="105" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="46"/>
@@ -10157,8 +10160,8 @@
       <c r="D105" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="E105" s="215"/>
-      <c r="F105" s="216"/>
+      <c r="E105" s="230"/>
+      <c r="F105" s="231"/>
     </row>
     <row r="106" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="46"/>
@@ -10169,8 +10172,8 @@
       <c r="D106" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="E106" s="215"/>
-      <c r="F106" s="216"/>
+      <c r="E106" s="230"/>
+      <c r="F106" s="231"/>
     </row>
     <row r="107" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="62"/>
@@ -10181,8 +10184,8 @@
       <c r="D107" s="83" t="s">
         <v>194</v>
       </c>
-      <c r="E107" s="225"/>
-      <c r="F107" s="226"/>
+      <c r="E107" s="216"/>
+      <c r="F107" s="217"/>
     </row>
     <row r="108" spans="1:6" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A108" s="84" t="s">
@@ -10369,6 +10372,13 @@
     <row r="122" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E102:F102"/>
     <mergeCell ref="E107:F107"/>
     <mergeCell ref="A66:F66"/>
     <mergeCell ref="E87:F87"/>
@@ -10385,13 +10395,6 @@
     <mergeCell ref="E103:F103"/>
     <mergeCell ref="E104:F104"/>
     <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="E102:F102"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.59" right="0.59" top="0.59" bottom="0.59" header="0.39000000000000007" footer="0.39000000000000007"/>
@@ -10704,10 +10707,10 @@
     <row r="23" spans="1:4" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="143"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="236" t="s">
+      <c r="C23" s="237" t="s">
         <v>892</v>
       </c>
-      <c r="D23" s="237"/>
+      <c r="D23" s="238"/>
     </row>
     <row r="24" spans="1:4" s="104" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="143"/>
@@ -10910,10 +10913,10 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="143"/>
       <c r="B45" s="18"/>
-      <c r="C45" s="235" t="s">
+      <c r="C45" s="236" t="s">
         <v>888</v>
       </c>
-      <c r="D45" s="235"/>
+      <c r="D45" s="236"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="143"/>
@@ -11608,89 +11611,89 @@
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="239"/>
-      <c r="B38" s="238"/>
+      <c r="B38" s="240"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
-      <c r="E38" s="238" t="s">
+      <c r="E38" s="240" t="s">
         <v>282</v>
       </c>
-      <c r="F38" s="238" t="s">
+      <c r="F38" s="240" t="s">
         <v>283</v>
       </c>
       <c r="G38" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="H38" s="238" t="s">
+      <c r="H38" s="240" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="239"/>
-      <c r="B39" s="238"/>
+      <c r="B39" s="240"/>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
-      <c r="E39" s="238"/>
-      <c r="F39" s="238"/>
+      <c r="E39" s="240"/>
+      <c r="F39" s="240"/>
       <c r="G39" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="H39" s="238"/>
+      <c r="H39" s="240"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="239"/>
-      <c r="B40" s="238"/>
+      <c r="B40" s="240"/>
       <c r="C40" s="25"/>
       <c r="D40" s="25"/>
-      <c r="E40" s="238" t="s">
+      <c r="E40" s="240" t="s">
         <v>287</v>
       </c>
-      <c r="F40" s="238" t="s">
+      <c r="F40" s="240" t="s">
         <v>288</v>
       </c>
-      <c r="G40" s="238" t="s">
+      <c r="G40" s="240" t="s">
         <v>289</v>
       </c>
-      <c r="H40" s="238" t="s">
+      <c r="H40" s="240" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="239"/>
-      <c r="B41" s="238"/>
+      <c r="B41" s="240"/>
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
-      <c r="E41" s="238"/>
-      <c r="F41" s="238"/>
-      <c r="G41" s="238"/>
-      <c r="H41" s="238"/>
+      <c r="E41" s="240"/>
+      <c r="F41" s="240"/>
+      <c r="G41" s="240"/>
+      <c r="H41" s="240"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="239"/>
-      <c r="B42" s="238"/>
+      <c r="B42" s="240"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
-      <c r="E42" s="238" t="s">
+      <c r="E42" s="240" t="s">
         <v>291</v>
       </c>
-      <c r="F42" s="238" t="s">
+      <c r="F42" s="240" t="s">
         <v>292</v>
       </c>
-      <c r="G42" s="238" t="s">
+      <c r="G42" s="240" t="s">
         <v>293</v>
       </c>
-      <c r="H42" s="238" t="s">
+      <c r="H42" s="240" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="239"/>
-      <c r="B43" s="238"/>
+      <c r="B43" s="240"/>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
-      <c r="E43" s="238"/>
-      <c r="F43" s="238"/>
-      <c r="G43" s="238"/>
-      <c r="H43" s="238"/>
+      <c r="E43" s="240"/>
+      <c r="F43" s="240"/>
+      <c r="G43" s="240"/>
+      <c r="H43" s="240"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="27" t="s">
@@ -11738,28 +11741,28 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="239"/>
-      <c r="B47" s="238"/>
+      <c r="B47" s="240"/>
       <c r="C47" s="25"/>
       <c r="D47" s="25"/>
-      <c r="E47" s="238" t="s">
+      <c r="E47" s="240" t="s">
         <v>301</v>
       </c>
-      <c r="F47" s="238" t="s">
+      <c r="F47" s="240" t="s">
         <v>302</v>
       </c>
-      <c r="G47" s="238"/>
+      <c r="G47" s="240"/>
       <c r="H47" s="25" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="239"/>
-      <c r="B48" s="238"/>
+      <c r="B48" s="240"/>
       <c r="C48" s="25"/>
       <c r="D48" s="25"/>
-      <c r="E48" s="238"/>
-      <c r="F48" s="238"/>
-      <c r="G48" s="238"/>
+      <c r="E48" s="240"/>
+      <c r="F48" s="240"/>
+      <c r="G48" s="240"/>
       <c r="H48" s="25" t="s">
         <v>304</v>
       </c>
@@ -11840,16 +11843,16 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="239"/>
-      <c r="B54" s="238"/>
+      <c r="B54" s="240"/>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
-      <c r="E54" s="238" t="s">
+      <c r="E54" s="240" t="s">
         <v>316</v>
       </c>
-      <c r="F54" s="238" t="s">
+      <c r="F54" s="240" t="s">
         <v>317</v>
       </c>
-      <c r="G54" s="238" t="s">
+      <c r="G54" s="240" t="s">
         <v>318</v>
       </c>
       <c r="H54" s="25" t="s">
@@ -11858,12 +11861,12 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="239"/>
-      <c r="B55" s="238"/>
+      <c r="B55" s="240"/>
       <c r="C55" s="25"/>
       <c r="D55" s="25"/>
-      <c r="E55" s="238"/>
-      <c r="F55" s="238"/>
-      <c r="G55" s="238"/>
+      <c r="E55" s="240"/>
+      <c r="F55" s="240"/>
+      <c r="G55" s="240"/>
       <c r="H55" s="25" t="s">
         <v>319</v>
       </c>
@@ -11948,6 +11951,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="G47:G48"/>
     <mergeCell ref="A54:A55"/>
@@ -11959,22 +11975,9 @@
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="E47:E48"/>
     <mergeCell ref="F47:F48"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="F38:F39"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="H40:H41"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.59" right="0.59" top="0.59" bottom="0.59" header="0.39000000000000007" footer="0.39000000000000007"/>
@@ -12102,12 +12105,12 @@
       <c r="D9" s="176"/>
     </row>
     <row r="11" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="240" t="s">
+      <c r="A11" s="241" t="s">
         <v>341</v>
       </c>
-      <c r="B11" s="240"/>
-      <c r="C11" s="240"/>
-      <c r="D11" s="240"/>
+      <c r="B11" s="241"/>
+      <c r="C11" s="241"/>
+      <c r="D11" s="241"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12128,10 +12131,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C54" sqref="C54"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12765,7 +12768,9 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="143"/>
       <c r="B54" s="149"/>
-      <c r="C54" s="151"/>
+      <c r="C54" s="151" t="s">
+        <v>973</v>
+      </c>
       <c r="D54" s="102" t="s">
         <v>454</v>
       </c>
@@ -12809,13 +12814,13 @@
       <c r="E57" s="21"/>
     </row>
     <row r="59" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="241" t="s">
+      <c r="A59" s="242" t="s">
         <v>841</v>
       </c>
-      <c r="B59" s="241"/>
-      <c r="C59" s="241"/>
-      <c r="D59" s="241"/>
-      <c r="E59" s="241"/>
+      <c r="B59" s="242"/>
+      <c r="C59" s="242"/>
+      <c r="D59" s="242"/>
+      <c r="E59" s="242"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13123,13 +13128,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="242" t="s">
+      <c r="A27" s="243" t="s">
         <v>963</v>
       </c>
-      <c r="B27" s="242"/>
-      <c r="C27" s="242"/>
-      <c r="D27" s="242"/>
-      <c r="E27" s="242"/>
+      <c r="B27" s="243"/>
+      <c r="C27" s="243"/>
+      <c r="D27" s="243"/>
+      <c r="E27" s="243"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13518,14 +13523,14 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="243" t="s">
+      <c r="A30" s="244" t="s">
         <v>803</v>
       </c>
-      <c r="B30" s="243"/>
-      <c r="C30" s="243"/>
-      <c r="D30" s="243"/>
-      <c r="E30" s="243"/>
-      <c r="F30" s="243"/>
+      <c r="B30" s="244"/>
+      <c r="C30" s="244"/>
+      <c r="D30" s="244"/>
+      <c r="E30" s="244"/>
+      <c r="F30" s="244"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>